<commit_message>
Test signal working at 4kHz.
</commit_message>
<xml_diff>
--- a/Ads1299_defRegs.xlsx
+++ b/Ads1299_defRegs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahmood31\Google Drive\nRF5_SDK_13.1.0\examples\_my_projects\nRF52_ADS1299_2CH_EEG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox (GaTech)\NRF\nRF5_SDK_13.1.0\examples\_my_projects\nRF52_ADS1299_EMG_kHz\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -712,7 +712,7 @@
   <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,16 +1005,16 @@
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
-        <v>0x61</v>
+        <v>0x05</v>
       </c>
       <c r="D7" s="11">
         <v>0</v>
       </c>
       <c r="E7" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" s="11">
         <v>0</v>
@@ -1023,7 +1023,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" s="11">
         <v>0</v>

</xml_diff>